<commit_message>
Image of current campain
</commit_message>
<xml_diff>
--- a/DnData/D20/MYLUCK_21Camp.xlsx
+++ b/DnData/D20/MYLUCK_21Camp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\DnData\D20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EFC56B-97F6-4A48-A43E-CA559073FE2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF73CC2-BF54-4FC4-AB82-10734455E3DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555EC10F-2DA9-4A2E-ABDF-A872F8AFBE1A}"/>
   </bookViews>
@@ -2703,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8EF6D9-5AD5-43CA-9518-DC5AA8E532CB}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
xslx update from ses
</commit_message>
<xml_diff>
--- a/DnData/D20/MYLUCK_21Camp.xlsx
+++ b/DnData/D20/MYLUCK_21Camp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\DnData\D20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF73CC2-BF54-4FC4-AB82-10734455E3DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208E7228-7EDF-4A1A-87A8-4B328B921BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555EC10F-2DA9-4A2E-ABDF-A872F8AFBE1A}"/>
   </bookViews>
@@ -312,7 +312,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>43</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>16</c:v>
@@ -321,7 +321,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
@@ -333,7 +333,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>11</c:v>
@@ -354,13 +354,13 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>19</c:v>
@@ -961,7 +961,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>43</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>16</c:v>
@@ -970,7 +970,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
@@ -982,7 +982,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>11</c:v>
@@ -1003,13 +1003,13 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>19</c:v>
@@ -2703,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8EF6D9-5AD5-43CA-9518-DC5AA8E532CB}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2734,11 +2734,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3">
         <f>B2/B22 * 100</f>
-        <v>13.479623824451412</v>
+        <v>14.110429447852759</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="C3" s="3">
         <f>B3/B22 * 100</f>
-        <v>5.0156739811912221</v>
+        <v>4.9079754601226995</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="C4" s="3">
         <f>B4/B22 * 100</f>
-        <v>4.0752351097178678</v>
+        <v>3.9877300613496933</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -2779,11 +2779,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3">
         <f>B5/B22 * 100</f>
-        <v>3.761755485893417</v>
+        <v>3.9877300613496933</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="C6" s="3">
         <f>B6/B22 * 100</f>
-        <v>5.0156739811912221</v>
+        <v>4.9079754601226995</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C7" s="3">
         <f>B7/B22 * 100</f>
-        <v>4.0752351097178678</v>
+        <v>3.9877300613496933</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="C8" s="3">
         <f>B8/B22 * 100</f>
-        <v>3.4482758620689653</v>
+        <v>3.3742331288343559</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -2839,11 +2839,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3">
         <f>B9/B22 * 100</f>
-        <v>4.0752351097178678</v>
+        <v>4.294478527607362</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="C10" s="3">
         <f>B10/B22 * 100</f>
-        <v>3.4482758620689653</v>
+        <v>3.3742331288343559</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="C11" s="3">
         <f>B11/B22 * 100</f>
-        <v>4.7021943573667713</v>
+        <v>4.6012269938650308</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C12" s="3">
         <f>B12/B22 * 100</f>
-        <v>5.6426332288401255</v>
+        <v>5.5214723926380369</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="C13" s="3">
         <f>B13/B22 * 100</f>
-        <v>4.7021943573667713</v>
+        <v>4.6012269938650308</v>
       </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="C14" s="3">
         <f>B14/B22 * 100</f>
-        <v>5.3291536050156738</v>
+        <v>5.2147239263803682</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -2933,7 +2933,7 @@
       </c>
       <c r="C15" s="3">
         <f>B15/B22 * 100</f>
-        <v>5.9561128526645764</v>
+        <v>5.8282208588957047</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2944,11 +2944,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="3">
         <f>B16/B22 * 100</f>
-        <v>4.3887147335423196</v>
+        <v>4.6012269938650308</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="C17" s="3">
         <f>B17/B22 * 100</f>
-        <v>5.0156739811912221</v>
+        <v>4.9079754601226995</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -2974,11 +2974,11 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3">
         <f>B18/B22 * 100</f>
-        <v>4.3887147335423196</v>
+        <v>4.6012269938650308</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="C19" s="3">
         <f>B19/B22 * 100</f>
-        <v>5.9561128526645764</v>
+        <v>5.8282208588957047</v>
       </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="C20" s="3">
         <f>B20/B22 * 100</f>
-        <v>4.0752351097178678</v>
+        <v>3.9877300613496933</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -3026,7 +3026,7 @@
       </c>
       <c r="C21" s="3">
         <f>B21/B22 * 100</f>
-        <v>3.4482758620689653</v>
+        <v>3.3742331288343559</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
@@ -3038,7 +3038,7 @@
       </c>
       <c r="B22">
         <f>SUM(B2:B21)</f>
-        <v>319</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
@@ -3050,11 +3050,11 @@
       </c>
       <c r="B24">
         <f>SUM(B2:B11)</f>
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C24" s="3">
         <f>SUM(C2:C11)</f>
-        <v>51.097178683385579</v>
+        <v>51.533742331288344</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
@@ -3063,11 +3063,11 @@
       </c>
       <c r="B25">
         <f>SUM(B12:B21)</f>
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C25" s="3">
         <f>SUM(C12:C21)</f>
-        <v>48.902821316614421</v>
+        <v>48.466257668711656</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Forgot to update roll stats earlier
</commit_message>
<xml_diff>
--- a/DnData/D20/MYLUCK_21Camp.xlsx
+++ b/DnData/D20/MYLUCK_21Camp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\DnData\D20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF55E9DF-9068-4DDD-AAB7-19EBA85065F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E98A89-E7D8-4CA3-AE71-21956FD16CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555EC10F-2DA9-4A2E-ABDF-A872F8AFBE1A}"/>
   </bookViews>
@@ -315,13 +315,13 @@
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>17</c:v>
@@ -342,7 +342,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>17</c:v>
@@ -351,7 +351,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>16</c:v>
@@ -360,13 +360,13 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>15</c:v>
@@ -964,13 +964,13 @@
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>17</c:v>
@@ -991,7 +991,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>17</c:v>
@@ -1000,7 +1000,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>16</c:v>
@@ -1009,13 +1009,13 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>15</c:v>
@@ -2703,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8EF6D9-5AD5-43CA-9518-DC5AA8E532CB}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="C2" s="3">
         <f>B2/B22 * 100</f>
-        <v>13.29639889196676</v>
+        <v>12.972972972972974</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -2749,11 +2749,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3">
         <f>B3/B22 * 100</f>
-        <v>4.43213296398892</v>
+        <v>4.8648648648648649</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -2764,11 +2764,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3">
         <f>B4/B22 * 100</f>
-        <v>3.8781163434903045</v>
+        <v>4.0540540540540544</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -2779,11 +2779,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
         <f>B5/B22 * 100</f>
-        <v>3.8781163434903045</v>
+        <v>4.0540540540540544</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="C6" s="3">
         <f>B6/B22 * 100</f>
-        <v>4.7091412742382275</v>
+        <v>4.5945945945945947</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C7" s="3">
         <f>B7/B22 * 100</f>
-        <v>4.1551246537396125</v>
+        <v>4.0540540540540544</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="C8" s="3">
         <f>B8/B22 * 100</f>
-        <v>4.43213296398892</v>
+        <v>4.3243243243243246</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -2843,7 +2843,7 @@
       </c>
       <c r="C9" s="3">
         <f>B9/B22 * 100</f>
-        <v>4.1551246537396125</v>
+        <v>4.0540540540540544</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="C10" s="3">
         <f>B10/B22 * 100</f>
-        <v>3.6011080332409975</v>
+        <v>3.5135135135135136</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="C11" s="3">
         <f>B11/B22 * 100</f>
-        <v>4.1551246537396125</v>
+        <v>4.0540540540540544</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -2884,11 +2884,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3">
         <f>B12/B22 * 100</f>
-        <v>6.094182825484765</v>
+        <v>6.4864864864864868</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="C13" s="3">
         <f>B13/B22 * 100</f>
-        <v>4.7091412742382275</v>
+        <v>4.5945945945945947</v>
       </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="C14" s="3">
         <f>B14/B22 * 100</f>
-        <v>4.986149584487535</v>
+        <v>4.8648648648648649</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -2929,11 +2929,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3">
         <f>B15/B22 * 100</f>
-        <v>5.5401662049861491</v>
+        <v>5.6756756756756763</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="C16" s="3">
         <f>B16/B22 * 100</f>
-        <v>4.43213296398892</v>
+        <v>4.3243243243243246</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="C17" s="3">
         <f>B17/B22 * 100</f>
-        <v>5.2631578947368416</v>
+        <v>5.1351351351351351</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -2974,11 +2974,11 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="3">
         <f>B18/B22 * 100</f>
-        <v>4.1551246537396125</v>
+        <v>4.3243243243243246</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="C19" s="3">
         <f>B19/B22 * 100</f>
-        <v>5.5401662049861491</v>
+        <v>5.4054054054054053</v>
       </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -3007,11 +3007,11 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="3">
         <f>B20/B22 * 100</f>
-        <v>4.43213296398892</v>
+        <v>4.5945945945945947</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -3026,7 +3026,7 @@
       </c>
       <c r="C21" s="3">
         <f>B21/B22 * 100</f>
-        <v>4.1551246537396125</v>
+        <v>4.0540540540540544</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
@@ -3038,7 +3038,7 @@
       </c>
       <c r="B22">
         <f>SUM(B2:B21)</f>
-        <v>361</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
@@ -3050,11 +3050,11 @@
       </c>
       <c r="B24">
         <f>SUM(B2:B11)</f>
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C24" s="3">
         <f>SUM(C2:C11)</f>
-        <v>50.692520775623272</v>
+        <v>50.540540540540555</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
@@ -3063,11 +3063,11 @@
       </c>
       <c r="B25">
         <f>SUM(B12:B21)</f>
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C25" s="3">
         <f>SUM(C12:C21)</f>
-        <v>49.307479224376735</v>
+        <v>49.45945945945946</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">

</xml_diff>